<commit_message>
Removed json database stuff
</commit_message>
<xml_diff>
--- a/data/nutrition.xlsx
+++ b/data/nutrition.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -408,9 +408,23 @@
         <v>calories</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>213_8290</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2022/01/23 13:41:26</v>
+      </c>
+      <c r="C2" t="str">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>